<commit_message>
edit lai wh2_pf. rm pf_da_eo, add wh2_pf_eo
</commit_message>
<xml_diff>
--- a/_linhtinh/file_linhtinh/reges_get_transaction.xlsx
+++ b/_linhtinh/file_linhtinh/reges_get_transaction.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\P&amp;G\my_project\_linhtinh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\P&amp;G\my_project\_linhtinh\file_linhtinh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B7834F-A25C-457F-95B2-F3021E4B3531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01773CFA-963C-4F10-A11A-70A0441D6DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{2916A480-0CB3-4E41-813B-B7E2FF749114}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="27852" windowHeight="16416" xr2:uid="{2916A480-0CB3-4E41-813B-B7E2FF749114}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="trans" sheetId="1" r:id="rId1"/>
+    <sheet name="tonkho" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">trans!$A$1:$C$6</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>lot và vn07</t>
   </si>
@@ -142,6 +143,18 @@
   </si>
   <si>
     <t>(?=.*?(?&lt;=[A-Z])(;\d+-\d{1}))(?=.*?(?&lt;=(?:\d{2}\/){2}\d{2})(;(?:\d{2}:){2}\d{2}))(?=.*?(?&lt;=(?:F|P))(;\d{2,20}))(?=.*?(?:\d+;)(?=[A-Z0-9]*))</t>
+  </si>
+  <si>
+    <t>regex lấy tồn kho PG</t>
+  </si>
+  <si>
+    <t>^(?:.+)(?&lt;=NONE)(?:\b)</t>
+  </si>
+  <si>
+    <t>regex lấy loại file</t>
+  </si>
+  <si>
+    <t>(?&lt;=Class:\s)(?:F|P)(?=\s+Item:)</t>
   </si>
 </sst>
 </file>
@@ -495,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2905127E-8D3D-442A-9DFE-C9BDED215ABE}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,4 +693,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9F4593-32E8-4D9B-8F23-CF77BF894055}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>